<commit_message>
Reformat code and added listeners with correct path.
</commit_message>
<xml_diff>
--- a/src/main/resources/reports/AutomationCoreReportTemplate.xlsx
+++ b/src/main/resources/reports/AutomationCoreReportTemplate.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hammer.hernandez/Documents/Repositories/automation-core-suite/src/main/resources/reports/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F738D9C1-AF79-4C45-A7C5-805DC0601B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -13,8 +19,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Results!$A$1:$I$3</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -109,7 +125,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
@@ -305,15 +321,15 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -581,7 +597,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4">
-    <tableStyle name="PivotCustomStyle" table="0" count="15">
+    <tableStyle name="PivotCustomStyle" table="0" count="15" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="14"/>
       <tableStyleElement type="headerRow" dxfId="13"/>
       <tableStyleElement type="totalRow" dxfId="12"/>
@@ -599,11 +615,19 @@
       <tableStyleElement type="pageFieldValues" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -617,7 +641,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -639,6 +662,11 @@
                 <a:srgbClr val="008000"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-F702-4442-9E76-3737059EA26B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -648,6 +676,11 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-F702-4442-9E76-3737059EA26B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -660,8 +693,20 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-F702-4442-9E76-3737059EA26B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -670,6 +715,9 @@
             <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -695,17 +743,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-F702-4442-9E76-3737059EA26B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="outEnd"/>
@@ -722,7 +775,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -731,7 +783,7 @@
           <a:pPr rtl="0">
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -741,7 +793,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -749,44 +801,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38333</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>7144</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="406400" y="38333"/>
-          <a:ext cx="4406900" cy="730811"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -802,7 +816,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -811,7 +831,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1141,47 +1161,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" customWidth="1"/>
     <col min="8" max="8" width="42.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="14"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
+      <c r="H2" s="17"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
       <c r="G3" t="s">
         <v>1</v>
       </c>
@@ -1189,21 +1209,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="7" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1212,7 +1232,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1221,7 +1241,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1230,13 +1250,13 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1245,7 +1265,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1254,7 +1274,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -1263,7 +1283,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1272,13 +1292,13 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
@@ -1286,22 +1306,22 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="30">
+    <row r="22" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="15" t="e">
+      <c r="B22" s="13" t="e">
         <f ca="1">AVERAGE(OFFSET(Results!$G$2,0,0,B21,1))</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>24</v>
       </c>
@@ -1327,12 +1347,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
@@ -1340,12 +1360,12 @@
     <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="24.33203125" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" style="13" customWidth="1"/>
     <col min="8" max="8" width="17.5" style="2" customWidth="1"/>
     <col min="9" max="9" width="18.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
@@ -1364,7 +1384,7 @@
       <c r="F1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="9" t="s">
@@ -1374,7 +1394,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>12</v>
       </c>
@@ -1393,7 +1413,7 @@
       <c r="F2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="15">
         <v>0</v>
       </c>
       <c r="H2" s="12">
@@ -1403,7 +1423,7 @@
         <v>42005</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>12</v>
       </c>
@@ -1422,7 +1442,7 @@
       <c r="F3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="15">
         <v>0</v>
       </c>
       <c r="H3" s="12">

</xml_diff>